<commit_message>
Updated worlog and added Research resource file
</commit_message>
<xml_diff>
--- a/Worklog_Anupam_220025208_SIT723.xlsx
+++ b/Worklog_Anupam_220025208_SIT723.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\offic\Documents\SIT723_T3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\offic\Documents\SIT723_T3\SIT723_T3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31900E72-115A-4E96-A3F3-92E86F616F23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{117CF31D-F8D5-44A1-8C10-339CF2FBA825}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{D01C876E-0C57-1449-A864-F752FD507052}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" state="hidden" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="39">
   <si>
     <t>Student Name</t>
   </si>
@@ -134,6 +134,24 @@
   </si>
   <si>
     <t>Human Research Ethics Training</t>
+  </si>
+  <si>
+    <t>Ontrack Task 1.1 Project Initiation and 1.2 Project in your own words</t>
+  </si>
+  <si>
+    <t>Task 1.2 Project in yur own words</t>
+  </si>
+  <si>
+    <t>Shared literature with supervisors and got their feedback.</t>
+  </si>
+  <si>
+    <t>Literature Search on AI cost, AI evaluation, ROI of software projects etc</t>
+  </si>
+  <si>
+    <t>Weekly Workshop Week 2</t>
+  </si>
+  <si>
+    <t>Total Hours</t>
   </si>
 </sst>
 </file>
@@ -530,10 +548,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBC54600-A529-144A-8AA1-058C0E013D1F}">
-  <dimension ref="A1:H13"/>
+  <dimension ref="A1:I20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -544,11 +562,11 @@
     <col min="4" max="4" width="21.19921875" customWidth="1"/>
     <col min="5" max="5" width="20.796875" customWidth="1"/>
     <col min="6" max="6" width="28.69921875" customWidth="1"/>
-    <col min="7" max="7" width="68.796875" customWidth="1"/>
+    <col min="7" max="7" width="87.69921875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="22.19921875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" ht="18" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -572,7 +590,7 @@
       </c>
       <c r="H1" s="2"/>
     </row>
-    <row r="2" spans="1:8" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>8</v>
       </c>
@@ -595,7 +613,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" ht="18" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>23</v>
       </c>
@@ -617,8 +635,11 @@
       <c r="G3" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I3" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>23</v>
       </c>
@@ -640,8 +661,12 @@
       <c r="G4" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I4">
+        <f>SUM(E3:E20)/60</f>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>23</v>
       </c>
@@ -664,7 +689,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>23</v>
       </c>
@@ -687,7 +712,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>23</v>
       </c>
@@ -710,7 +735,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>23</v>
       </c>
@@ -733,7 +758,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>23</v>
       </c>
@@ -756,7 +781,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>23</v>
       </c>
@@ -779,7 +804,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>23</v>
       </c>
@@ -802,7 +827,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>23</v>
       </c>
@@ -825,7 +850,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>23</v>
       </c>
@@ -839,13 +864,174 @@
         <v>44519</v>
       </c>
       <c r="E13">
-        <v>120</v>
+        <v>60</v>
       </c>
       <c r="F13" t="s">
+        <v>14</v>
+      </c>
+      <c r="G13" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>23</v>
+      </c>
+      <c r="B14" t="s">
+        <v>24</v>
+      </c>
+      <c r="C14" t="s">
+        <v>25</v>
+      </c>
+      <c r="D14" s="4">
+        <v>44519</v>
+      </c>
+      <c r="E14">
+        <v>120</v>
+      </c>
+      <c r="F14" t="s">
         <v>15</v>
       </c>
-      <c r="G13" t="s">
+      <c r="G14" t="s">
         <v>32</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>23</v>
+      </c>
+      <c r="B15" t="s">
+        <v>24</v>
+      </c>
+      <c r="C15" t="s">
+        <v>25</v>
+      </c>
+      <c r="D15" s="4">
+        <v>44520</v>
+      </c>
+      <c r="E15">
+        <v>120</v>
+      </c>
+      <c r="F15" t="s">
+        <v>15</v>
+      </c>
+      <c r="G15" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>23</v>
+      </c>
+      <c r="B16" t="s">
+        <v>24</v>
+      </c>
+      <c r="C16" t="s">
+        <v>25</v>
+      </c>
+      <c r="D16" s="4">
+        <v>44521</v>
+      </c>
+      <c r="E16">
+        <v>120</v>
+      </c>
+      <c r="F16" t="s">
+        <v>11</v>
+      </c>
+      <c r="G16" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>23</v>
+      </c>
+      <c r="B17" t="s">
+        <v>24</v>
+      </c>
+      <c r="C17" t="s">
+        <v>25</v>
+      </c>
+      <c r="D17" s="4">
+        <v>44522</v>
+      </c>
+      <c r="E17">
+        <v>120</v>
+      </c>
+      <c r="F17" t="s">
+        <v>15</v>
+      </c>
+      <c r="G17" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>23</v>
+      </c>
+      <c r="B18" t="s">
+        <v>24</v>
+      </c>
+      <c r="C18" t="s">
+        <v>25</v>
+      </c>
+      <c r="D18" s="4">
+        <v>44525</v>
+      </c>
+      <c r="E18">
+        <v>120</v>
+      </c>
+      <c r="F18" t="s">
+        <v>14</v>
+      </c>
+      <c r="G18" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>23</v>
+      </c>
+      <c r="B19" t="s">
+        <v>24</v>
+      </c>
+      <c r="C19" t="s">
+        <v>25</v>
+      </c>
+      <c r="D19" s="4">
+        <v>44525</v>
+      </c>
+      <c r="E19">
+        <v>120</v>
+      </c>
+      <c r="F19" t="s">
+        <v>11</v>
+      </c>
+      <c r="G19" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>23</v>
+      </c>
+      <c r="B20" t="s">
+        <v>24</v>
+      </c>
+      <c r="C20" t="s">
+        <v>25</v>
+      </c>
+      <c r="D20" s="4">
+        <v>44526</v>
+      </c>
+      <c r="E20">
+        <v>60</v>
+      </c>
+      <c r="F20" t="s">
+        <v>14</v>
+      </c>
+      <c r="G20" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -857,7 +1043,7 @@
           <x14:formula1>
             <xm:f>Sheet2!$A$1:$A$12</xm:f>
           </x14:formula1>
-          <xm:sqref>E3:E432</xm:sqref>
+          <xm:sqref>E3:E433</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{A18E5B6F-7CCC-C74F-9785-6997C435583D}">
           <x14:formula1>
@@ -992,6 +1178,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010082532935BEA4414DAD83A5DF5EC08D50" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="1fab9b1b639c92c05cfd4aa2b4bf08c0">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="ffdfa1cc-c946-49f6-99ef-ff4ab350a4c7" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="cad3acc22b2eb44b3a116b77879253d7" ns2:_="">
     <xsd:import namespace="ffdfa1cc-c946-49f6-99ef-ff4ab350a4c7"/>
@@ -1123,15 +1318,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{33C84895-33C6-4EEF-ADE3-B2C6A0E7CE9B}">
   <ds:schemaRefs>
@@ -1142,6 +1328,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{99F33CB9-EBB9-4740-8AC2-6F0A2CE058F7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9FF34756-59E0-48B0-8E6C-773EF7EF3DA4}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1157,12 +1351,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{99F33CB9-EBB9-4740-8AC2-6F0A2CE058F7}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>